<commit_message>
minor fixing unit of measure
</commit_message>
<xml_diff>
--- a/Scenarios/a_Traditional-Energy-System/Results/EnergySystemSize.xlsx
+++ b/Scenarios/a_Traditional-Energy-System/Results/EnergySystemSize.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Documenti\GitHub\MicroGridsPy-MultiEnergy_Paper\Scenarios\a_Traditional-Energy-System\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE6B39-CF04-457A-AE3E-FC4DD2FCF606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="585" windowWidth="17895" windowHeight="8385" activeTab="2"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="21600" windowHeight="11205" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Size" sheetId="1" r:id="rId1"/>
@@ -120,8 +126,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +193,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -476,20 +485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -532,10 +540,10 @@
         <v>9</v>
       </c>
       <c r="G2">
-        <v>0.181613</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>181.613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -543,19 +551,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.24492256847153379</v>
+        <v>0.24498372462774901</v>
       </c>
       <c r="D3">
-        <v>1.0691500829924681</v>
+        <v>1.069245166222947</v>
       </c>
       <c r="E3">
-        <v>5.4702348647308781E-2</v>
+        <v>5.4720253761115452E-2</v>
       </c>
       <c r="F3">
-        <v>4.7437039778911852E-2</v>
+        <v>4.7441902205855001E-2</v>
       </c>
       <c r="G3">
-        <v>1.4162120398902229</v>
+        <v>1.4163910468176659</v>
       </c>
     </row>
   </sheetData>
@@ -564,12 +572,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -578,7 +586,7 @@
     <col min="5" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -607,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -633,10 +641,10 @@
         <v>9</v>
       </c>
       <c r="I2">
-        <v>11.727617000862701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>11.727660594589549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -665,7 +673,7 @@
         <v>3.6322599999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -677,22 +685,22 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <v>2.4492256847153379E-2</v>
+        <v>2.4498372462774899E-2</v>
       </c>
       <c r="F4">
-        <v>0.1069150082992469</v>
+        <v>0.1069245166222946</v>
       </c>
       <c r="G4">
-        <v>5.4702348647308781E-3</v>
+        <v>5.4720253761115457E-3</v>
       </c>
       <c r="H4">
-        <v>4.7437039778911849E-3</v>
+        <v>4.7441902205855001E-3</v>
       </c>
       <c r="I4">
-        <v>0.14162120398902231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.1416391046817666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -721,7 +729,7 @@
         <v>5.0701282906726222E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -733,22 +741,22 @@
         <v>15</v>
       </c>
       <c r="E6">
-        <v>5.1281661146162141E-3</v>
+        <v>5.1294465965659201E-3</v>
       </c>
       <c r="F6">
-        <v>2.238576567793233E-2</v>
+        <v>2.2387756521829019E-2</v>
       </c>
       <c r="G6">
-        <v>1.145352723000105E-3</v>
+        <v>1.145727618619054E-3</v>
       </c>
       <c r="H6">
-        <v>9.9323235702630146E-4</v>
+        <v>9.933341660724839E-4</v>
       </c>
       <c r="I6">
-        <v>2.965251687257495E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>2.9656264903086479E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -774,10 +782,10 @@
         <v>9</v>
       </c>
       <c r="I7">
-        <v>3.765025902648707</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>3.7650259026486861</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -789,22 +797,22 @@
         <v>15</v>
       </c>
       <c r="E8">
-        <v>1.93344567191026</v>
+        <v>1.9334530857065171</v>
       </c>
       <c r="F8">
-        <v>5.6675340018190417</v>
+        <v>5.667545708009242</v>
       </c>
       <c r="G8">
-        <v>8.2657535828159254E-2</v>
+        <v>8.2659778913065252E-2</v>
       </c>
       <c r="H8">
-        <v>2.0656284888202509E-2</v>
+        <v>2.065686682046405E-2</v>
       </c>
       <c r="I8">
-        <v>7.7042934944456638</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>7.7043154394492879</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -833,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -873,19 +881,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
@@ -896,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -904,16 +912,16 @@
         <v>26</v>
       </c>
       <c r="C2">
-        <v>159.2473803333333</v>
+        <v>159247.38033333331</v>
       </c>
       <c r="D2">
-        <v>167.22101343010351</v>
+        <v>167221.48974450849</v>
       </c>
       <c r="E2">
-        <v>326.46839376343678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>326468.8700778418</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -930,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -947,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -955,16 +963,16 @@
         <v>28</v>
       </c>
       <c r="C5">
-        <v>0.3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="D5">
-        <v>0.87878787878787867</v>
+        <v>8.7878537564473449E-4</v>
       </c>
       <c r="E5">
-        <v>0.59646206953222236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>5.9646119930077983E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -978,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>258.8779320853086</v>
+        <v>0.25887889438258183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a&b in kW w/ results
</commit_message>
<xml_diff>
--- a/Scenarios/a_Traditional-Energy-System/Results/EnergySystemSize.xlsx
+++ b/Scenarios/a_Traditional-Energy-System/Results/EnergySystemSize.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive\Documenti\GitHub\MicroGridsPy-MultiEnergy_Paper\Scenarios\a_Traditional-Energy-System\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AE6B39-CF04-457A-AE3E-FC4DD2FCF606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC01F66-5A73-4093-AB1D-1FFC4E1244B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="21600" windowHeight="11205" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Size" sheetId="1" r:id="rId1"/>
@@ -490,14 +490,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -543,7 +543,7 @@
         <v>181.613</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -551,19 +551,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>0.24498372462774901</v>
+        <v>244.98372462774901</v>
       </c>
       <c r="D3">
-        <v>1.069245166222947</v>
+        <v>1069.245166222946</v>
       </c>
       <c r="E3">
-        <v>5.4720253761115452E-2</v>
+        <v>54.720253761115451</v>
       </c>
       <c r="F3">
-        <v>4.7441902205855001E-2</v>
+        <v>47.441902205855001</v>
       </c>
       <c r="G3">
-        <v>1.4163910468176659</v>
+        <v>1416.3910468176659</v>
       </c>
     </row>
   </sheetData>
@@ -577,16 +577,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -615,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -644,7 +644,7 @@
         <v>11.727660594589549</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -673,7 +673,7 @@
         <v>3.6322599999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -700,7 +700,7 @@
         <v>0.1416391046817666</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -729,7 +729,7 @@
         <v>5.0701282906726222E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -756,7 +756,7 @@
         <v>2.9656264903086479E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -785,7 +785,7 @@
         <v>3.7650259026486861</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -812,7 +812,7 @@
         <v>7.7043154394492879</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -886,14 +886,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
@@ -904,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -921,7 +921,7 @@
         <v>326468.8700778418</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -938,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -963,16 +963,16 @@
         <v>28</v>
       </c>
       <c r="C5">
-        <v>2.9999999999999997E-4</v>
+        <v>0.3</v>
       </c>
       <c r="D5">
-        <v>8.7878537564473449E-4</v>
+        <v>0.87878537564473458</v>
       </c>
       <c r="E5">
-        <v>5.9646119930077983E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.59646119930077979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -986,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>0.25887889438258183</v>
+        <v>2.5887889438258192E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>